<commit_message>
se agregan excel resultados
</commit_message>
<xml_diff>
--- a/Proyecto/results/results_random_comparisson_stats.xlsx
+++ b/Proyecto/results/results_random_comparisson_stats.xlsx
@@ -462,34 +462,34 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>0.0006321456697252061</v>
+        <v>0.02416105270385742</v>
       </c>
       <c r="D2">
-        <v>0.0009946823120117188</v>
+        <v>0.0009993314743041992</v>
       </c>
       <c r="E2">
-        <v>0.0005062700847361874</v>
+        <v>0.1463630272162325</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2">
-        <v>0.001991987228393555</v>
+        <v>1.308655500411987</v>
       </c>
       <c r="H2">
-        <v>24530.96666666667</v>
+        <v>24563.41111111111</v>
       </c>
       <c r="I2">
-        <v>2978.678133978677</v>
+        <v>3515.979627244874</v>
       </c>
       <c r="J2">
-        <v>20612</v>
+        <v>19640</v>
       </c>
       <c r="K2">
-        <v>40820</v>
+        <v>44112</v>
       </c>
       <c r="L2">
-        <v>67.77777777777779</v>
+        <v>38.88888888888889</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -500,34 +500,34 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>0.0007333861456976996</v>
+        <v>2.233684341112772</v>
       </c>
       <c r="D3">
-        <v>0.0009993314743041992</v>
+        <v>0.003000259399414062</v>
       </c>
       <c r="E3">
-        <v>0.0004920870434928581</v>
+        <v>6.64942394537654</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3">
-        <v>0.001998186111450195</v>
+        <v>40.04736518859863</v>
       </c>
       <c r="H3">
-        <v>35358.02222222222</v>
+        <v>36717.41111111111</v>
       </c>
       <c r="I3">
-        <v>6193.984132826212</v>
+        <v>7129.612093541244</v>
       </c>
       <c r="J3">
-        <v>23036</v>
+        <v>22108</v>
       </c>
       <c r="K3">
-        <v>64556</v>
+        <v>76947</v>
       </c>
       <c r="L3">
-        <v>67.77777777777779</v>
+        <v>17.77777777777778</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -538,34 +538,34 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>0.001520927747090658</v>
+        <v>1.036487452189128</v>
       </c>
       <c r="D4">
-        <v>0.001000881195068359</v>
+        <v>0.003000020980834961</v>
       </c>
       <c r="E4">
-        <v>0.001151648862757556</v>
+        <v>3.269304157509965</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.00400090217590332</v>
+        <v>16.5603973865509</v>
       </c>
       <c r="H4">
-        <v>27558.7</v>
+        <v>27487.94444444445</v>
       </c>
       <c r="I4">
-        <v>4330.091738006318</v>
+        <v>4786.790405912643</v>
       </c>
       <c r="J4">
         <v>21608</v>
       </c>
       <c r="K4">
-        <v>45144</v>
+        <v>49248</v>
       </c>
       <c r="L4">
-        <v>67.77777777777779</v>
+        <v>38.88888888888889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>